<commit_message>
Support for loading Excel files #136
.. preserve ordering of sheets in the load result
</commit_message>
<xml_diff>
--- a/dflib-excel/src/test/resources/com/nhl/dflib/excel/multi-sheet.xlsx
+++ b/dflib-excel/src/test/resources/com/nhl/dflib/excel/multi-sheet.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrus/work/dflib/dflib/dflib-excel/src/test/resources/com/nhl/dflib/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777FEDDE-F59E-3142-804D-4F3F5A89CFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB1087D-C28C-7A47-BE71-769FBBECFFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27420" windowHeight="16940" activeTab="1" xr2:uid="{0F924BC7-E1FB-204E-9AE6-81BC34207CFC}"/>
   </bookViews>
   <sheets>
-    <sheet name="S1" sheetId="1" r:id="rId1"/>
-    <sheet name="S2" sheetId="2" r:id="rId2"/>
+    <sheet name="S2" sheetId="2" r:id="rId1"/>
+    <sheet name="S0" sheetId="3" r:id="rId2"/>
+    <sheet name="Some Sheet" sheetId="4" r:id="rId3"/>
+    <sheet name="S1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>One</t>
   </si>
@@ -59,6 +61,9 @@
   </si>
   <si>
     <t>Eight</t>
+  </si>
+  <si>
+    <t>SX</t>
   </si>
 </sst>
 </file>
@@ -409,6 +414,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F444F37-A648-7047-8D91-08D9C5A71172}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C989DC-AF11-E14E-87BD-029245C2CD87}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D04D27EF-47CD-2942-A71D-F50887E365FE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FC7934-7AFB-DF47-BEBF-D339A1CAABD0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -437,33 +503,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F444F37-A648-7047-8D91-08D9C5A71172}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>